<commit_message>
Update Rabu Malam 21-06-2023
</commit_message>
<xml_diff>
--- a/database_email.xlsx
+++ b/database_email.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasir\Documents\Coding\EMAIL DIESNAY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772F84B3-88BF-4FD4-889D-0CB258350669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980BAC8F-68D6-43FE-A51A-2F3AD8878581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2917E14B-08C0-4BCE-9B18-6DA83FE718B5}"/>
+    <workbookView xWindow="4884" yWindow="3060" windowWidth="17280" windowHeight="8880" xr2:uid="{2917E14B-08C0-4BCE-9B18-6DA83FE718B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Alamat Email</t>
   </si>
@@ -45,16 +45,10 @@
     <t>Status Pengiriman</t>
   </si>
   <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
     <t>Test 1</t>
   </si>
   <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>Test 2</t>
+    <t>akuntumbalknox@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -417,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41F0920-5D2F-4396-BBA0-C8C4AA00CE7C}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,27 +437,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{8B18FFE0-6C50-4200-A2A9-AC660D27E6F5}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{879290F2-691D-4940-B8D7-7E2077D4ECC9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>